<commit_message>
Configure React app for deployment to GitHub Pages
</commit_message>
<xml_diff>
--- a/public/Autism Information and Resources Offline.xlsx
+++ b/public/Autism Information and Resources Offline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CJ\Documents\My Projects\React_Practice\autism-resource-library\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BA98DC-24E8-444C-A3E5-FFA36F4521A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D94C6E4-B399-46FD-A3B0-2C1C25D0A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2616" yWindow="1104" windowWidth="20424" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -2558,7 +2558,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2608,14 +2608,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3191,10 +3184,10 @@
   <dimension ref="A1:T86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="T2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
+      <selection pane="bottomRight" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3479,7 +3472,7 @@
       <c r="F5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="35" t="s">
         <v>44</v>
       </c>
       <c r="H5" s="11" t="s">
@@ -4533,7 +4526,7 @@
       <c r="N22" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="O22" s="40" t="s">
+      <c r="O22" s="8" t="s">
         <v>174</v>
       </c>
       <c r="P22" s="1" t="s">
@@ -4562,7 +4555,7 @@
       <c r="C23" s="12" t="s">
         <v>573</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="12" t="s">
@@ -4680,12 +4673,12 @@
       <c r="C25" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="28" t="s">
         <v>42</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
-      <c r="G25" s="36"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="11" t="s">
         <v>182</v>
       </c>
@@ -4703,7 +4696,7 @@
       </c>
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="40" t="s">
+      <c r="O25" s="8" t="s">
         <v>185</v>
       </c>
       <c r="P25" s="1" t="s">
@@ -4732,7 +4725,7 @@
       <c r="C26" s="24" t="s">
         <v>573</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" t="s">
         <v>20</v>
       </c>
       <c r="E26" s="24" t="s">
@@ -4786,42 +4779,42 @@
       <c r="A27" s="10">
         <v>26</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="F27" s="36" t="e">
+      <c r="F27" s="28" t="e">
         <v>#N/A</v>
       </c>
-      <c r="G27" s="36" t="e">
+      <c r="G27" s="28" t="e">
         <v>#N/A</v>
       </c>
-      <c r="H27" s="36" t="s">
+      <c r="H27" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="I27" s="39">
+      <c r="I27" s="29">
         <v>8002</v>
       </c>
-      <c r="J27" s="36" t="s">
+      <c r="J27" s="28" t="s">
         <v>190</v>
       </c>
       <c r="K27" s="8" t="s">
         <v>494</v>
       </c>
-      <c r="L27" s="36" t="s">
+      <c r="L27" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="M27" s="36"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="40" t="s">
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="8" t="s">
         <v>220</v>
       </c>
       <c r="P27" s="1" t="s">
@@ -4835,7 +4828,7 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S27" s="36"/>
+      <c r="S27" s="28"/>
       <c r="T27" t="s">
         <v>707</v>
       </c>
@@ -4844,42 +4837,42 @@
       <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="36" t="s">
+      <c r="F28" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="G28" s="36" t="s">
+      <c r="G28" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="H28" s="36" t="s">
+      <c r="H28" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="I28" s="39">
+      <c r="I28" s="29">
         <v>7102</v>
       </c>
-      <c r="J28" s="36" t="s">
+      <c r="J28" s="28" t="s">
         <v>195</v>
       </c>
       <c r="K28" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="L28" s="36" t="s">
+      <c r="L28" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="M28" s="36"/>
-      <c r="N28" s="36"/>
-      <c r="O28" s="40" t="s">
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="8" t="s">
         <v>220</v>
       </c>
       <c r="P28" s="1" t="s">
@@ -4893,43 +4886,43 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S28" s="36"/>
+      <c r="S28" s="28"/>
     </row>
     <row r="29" spans="1:20" ht="115.2">
       <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="28" t="s">
         <v>187</v>
       </c>
       <c r="D29" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="E29" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36" t="s">
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="I29" s="39">
+      <c r="I29" s="29">
         <v>8542</v>
       </c>
-      <c r="J29" s="36" t="s">
+      <c r="J29" s="28" t="s">
         <v>198</v>
       </c>
       <c r="K29" s="8" t="s">
         <v>464</v>
       </c>
-      <c r="L29" s="36" t="s">
+      <c r="L29" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="M29" s="36"/>
-      <c r="N29" s="36"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
       <c r="O29" s="8" t="s">
         <v>220</v>
       </c>
@@ -4944,7 +4937,7 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S29" s="36"/>
+      <c r="S29" s="28"/>
       <c r="T29" t="s">
         <v>709</v>
       </c>
@@ -4953,41 +4946,40 @@
       <c r="A30" s="10">
         <v>29</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" t="s">
         <v>625</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" t="s">
         <v>573</v>
       </c>
       <c r="D30" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" t="s">
         <v>87</v>
       </c>
-      <c r="F30" s="35" t="s">
+      <c r="F30" t="s">
         <v>626</v>
       </c>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35" t="s">
+      <c r="H30" t="s">
         <v>627</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I30" s="2">
         <v>7109</v>
       </c>
-      <c r="J30" s="35" t="s">
+      <c r="J30" t="s">
         <v>628</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>629</v>
       </c>
-      <c r="L30" s="35" t="s">
+      <c r="L30" t="s">
         <v>630</v>
       </c>
-      <c r="M30" s="35" t="s">
+      <c r="M30" t="s">
         <v>631</v>
       </c>
-      <c r="N30" s="35" t="s">
+      <c r="N30" t="s">
         <v>632</v>
       </c>
       <c r="O30" s="8" t="s">
@@ -5002,7 +4994,6 @@
       <c r="R30">
         <v>21</v>
       </c>
-      <c r="S30" s="35"/>
       <c r="T30" t="s">
         <v>750</v>
       </c>
@@ -5066,26 +5057,26 @@
       <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="36" t="s">
+      <c r="E32" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="36" t="s">
+      <c r="F32" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36" t="s">
+      <c r="G32" s="28"/>
+      <c r="H32" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="I32" s="39">
+      <c r="I32" s="29">
         <v>7662</v>
       </c>
       <c r="J32" s="30" t="s">
@@ -5094,12 +5085,12 @@
       <c r="K32" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="L32" s="36" t="s">
+      <c r="L32" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="M32" s="36"/>
-      <c r="N32" s="36"/>
-      <c r="O32" s="40" t="s">
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="8" t="s">
         <v>220</v>
       </c>
       <c r="P32" s="1" t="s">
@@ -5113,7 +5104,7 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S32" s="36"/>
+      <c r="S32" s="28"/>
       <c r="T32" t="s">
         <v>758</v>
       </c>
@@ -5122,41 +5113,40 @@
       <c r="A33" s="10">
         <v>32</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" t="s">
         <v>616</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" t="s">
         <v>617</v>
       </c>
       <c r="D33" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" t="s">
         <v>344</v>
       </c>
-      <c r="F33" s="35" t="s">
+      <c r="F33" t="s">
         <v>618</v>
       </c>
-      <c r="G33" s="35"/>
-      <c r="H33" s="35" t="s">
+      <c r="H33" t="s">
         <v>619</v>
       </c>
-      <c r="I33" s="38">
+      <c r="I33" s="2">
         <v>8302</v>
       </c>
-      <c r="J33" s="35" t="s">
+      <c r="J33" t="s">
         <v>620</v>
       </c>
       <c r="K33" s="8" t="s">
         <v>621</v>
       </c>
-      <c r="L33" s="35" t="s">
+      <c r="L33" t="s">
         <v>622</v>
       </c>
-      <c r="M33" s="35" t="s">
+      <c r="M33" t="s">
         <v>623</v>
       </c>
-      <c r="N33" s="35" t="s">
+      <c r="N33" t="s">
         <v>624</v>
       </c>
       <c r="O33" s="8" t="s">
@@ -5171,7 +5161,6 @@
       <c r="R33">
         <v>21</v>
       </c>
-      <c r="S33" s="35"/>
       <c r="T33" t="s">
         <v>749</v>
       </c>
@@ -5180,40 +5169,37 @@
       <c r="A34" s="10">
         <v>33</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" t="s">
         <v>221</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" t="s">
         <v>187</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" t="s">
         <v>230</v>
       </c>
-      <c r="F34" s="35" t="s">
+      <c r="F34" t="s">
         <v>227</v>
       </c>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35" t="s">
+      <c r="H34" t="s">
         <v>228</v>
       </c>
-      <c r="I34" s="38">
+      <c r="I34" s="2">
         <v>8096</v>
       </c>
-      <c r="J34" s="35" t="s">
+      <c r="J34" t="s">
         <v>223</v>
       </c>
       <c r="K34" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="L34" s="35" t="s">
+      <c r="L34" t="s">
         <v>225</v>
       </c>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="40" t="s">
+      <c r="O34" s="8" t="s">
         <v>220</v>
       </c>
       <c r="P34" s="1" t="s">
@@ -5227,7 +5213,6 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S34" s="35"/>
       <c r="T34" t="s">
         <v>711</v>
       </c>
@@ -5294,28 +5279,28 @@
       <c r="A36" s="10">
         <v>35</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" t="s">
         <v>222</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" t="s">
         <v>187</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="36" t="s">
+      <c r="E36" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="35" t="s">
+      <c r="F36" t="s">
         <v>229</v>
       </c>
-      <c r="G36" s="35" t="s">
+      <c r="G36" t="s">
         <v>54</v>
       </c>
-      <c r="H36" s="35" t="s">
+      <c r="H36" t="s">
         <v>55</v>
       </c>
-      <c r="I36" s="38">
+      <c r="I36" s="2">
         <v>8520</v>
       </c>
       <c r="J36" s="33" t="s">
@@ -5324,11 +5309,9 @@
       <c r="K36" s="8" t="s">
         <v>468</v>
       </c>
-      <c r="L36" s="35" t="s">
+      <c r="L36" t="s">
         <v>226</v>
       </c>
-      <c r="M36" s="35"/>
-      <c r="N36" s="35"/>
       <c r="O36" s="8" t="s">
         <v>220</v>
       </c>
@@ -5343,7 +5326,6 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S36" s="35"/>
       <c r="T36" t="s">
         <v>712</v>
       </c>
@@ -5361,7 +5343,7 @@
       <c r="D37" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E37" t="s">
         <v>87</v>
       </c>
       <c r="F37" t="s">
@@ -5410,38 +5392,36 @@
       <c r="A38" s="10">
         <v>37</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" t="s">
         <v>231</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C38" t="s">
         <v>187</v>
       </c>
       <c r="D38" t="s">
         <v>20</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E38" t="s">
         <v>236</v>
       </c>
-      <c r="F38" s="35" t="s">
+      <c r="F38" t="s">
         <v>234</v>
       </c>
-      <c r="H38" s="35" t="s">
+      <c r="H38" t="s">
         <v>235</v>
       </c>
-      <c r="I38" s="38">
+      <c r="I38" s="2">
         <v>7202</v>
       </c>
-      <c r="J38" s="35" t="s">
+      <c r="J38" t="s">
         <v>232</v>
       </c>
       <c r="K38" s="8" t="s">
         <v>469</v>
       </c>
-      <c r="L38" s="35" t="s">
+      <c r="L38" t="s">
         <v>233</v>
       </c>
-      <c r="M38" s="35"/>
-      <c r="N38" s="35"/>
       <c r="O38" s="8" t="s">
         <v>220</v>
       </c>
@@ -5456,7 +5436,6 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S38" s="35"/>
       <c r="T38" t="s">
         <v>713</v>
       </c>
@@ -6377,36 +6356,31 @@
       <c r="A55" s="10">
         <v>54</v>
       </c>
-      <c r="B55" s="35" t="s">
+      <c r="B55" t="s">
         <v>411</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="C55" t="s">
         <v>41</v>
       </c>
-      <c r="D55" s="35" t="s">
+      <c r="D55" t="s">
         <v>42</v>
       </c>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="35"/>
-      <c r="I55" s="38"/>
-      <c r="J55" s="35" t="s">
+      <c r="J55" t="s">
         <v>417</v>
       </c>
       <c r="K55" s="8" t="s">
         <v>490</v>
       </c>
-      <c r="L55" s="35" t="s">
+      <c r="L55" t="s">
         <v>418</v>
       </c>
-      <c r="M55" s="35" t="s">
+      <c r="M55" t="s">
         <v>419</v>
       </c>
-      <c r="N55" s="35" t="s">
+      <c r="N55" t="s">
         <v>420</v>
       </c>
-      <c r="O55" s="40" t="s">
+      <c r="O55" s="8" t="s">
         <v>421</v>
       </c>
       <c r="P55" s="1" t="s">
@@ -6420,7 +6394,7 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S55" s="35" t="s">
+      <c r="S55" t="s">
         <v>412</v>
       </c>
       <c r="T55" t="s">
@@ -6431,33 +6405,28 @@
       <c r="A56" s="10">
         <v>55</v>
       </c>
-      <c r="B56" s="35" t="s">
+      <c r="B56" t="s">
         <v>413</v>
       </c>
-      <c r="C56" s="35" t="s">
+      <c r="C56" t="s">
         <v>176</v>
       </c>
-      <c r="D56" s="35" t="s">
+      <c r="D56" t="s">
         <v>42</v>
       </c>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="H56" s="35" t="s">
+      <c r="H56" t="s">
         <v>182</v>
       </c>
-      <c r="I56" s="38">
+      <c r="I56" s="2">
         <v>20035</v>
       </c>
-      <c r="J56" s="35" t="s">
+      <c r="J56" t="s">
         <v>183</v>
       </c>
       <c r="K56" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="L56" s="35"/>
-      <c r="M56" s="35"/>
-      <c r="N56" s="35"/>
-      <c r="O56" s="40" t="s">
+      <c r="O56" s="8" t="s">
         <v>422</v>
       </c>
       <c r="P56" s="1" t="s">
@@ -6471,7 +6440,6 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S56" s="35"/>
       <c r="T56" t="s">
         <v>761</v>
       </c>
@@ -6591,42 +6559,40 @@
       <c r="A59" s="10">
         <v>58</v>
       </c>
-      <c r="B59" s="35" t="s">
+      <c r="B59" t="s">
         <v>415</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C59" t="s">
         <v>176</v>
       </c>
-      <c r="D59" s="35" t="s">
+      <c r="D59" t="s">
         <v>42</v>
       </c>
-      <c r="E59" s="35" t="s">
+      <c r="E59" t="s">
         <v>434</v>
       </c>
-      <c r="F59" s="35" t="s">
+      <c r="F59" t="s">
         <v>430</v>
       </c>
-      <c r="G59" s="35" t="s">
+      <c r="G59" t="s">
         <v>431</v>
       </c>
-      <c r="H59" s="35" t="s">
+      <c r="H59" t="s">
         <v>432</v>
       </c>
-      <c r="I59" s="38">
+      <c r="I59" s="2">
         <v>20852</v>
       </c>
-      <c r="J59" s="35" t="s">
+      <c r="J59" t="s">
         <v>429</v>
       </c>
       <c r="K59" s="8" t="s">
         <v>685</v>
       </c>
-      <c r="L59" s="35" t="s">
+      <c r="L59" t="s">
         <v>433</v>
       </c>
-      <c r="M59" s="35"/>
-      <c r="N59" s="35"/>
-      <c r="O59" s="40" t="s">
+      <c r="O59" s="8" t="s">
         <v>422</v>
       </c>
       <c r="P59" s="1" t="s">
@@ -6640,7 +6606,6 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S59" s="35"/>
       <c r="T59" t="s">
         <v>706</v>
       </c>
@@ -6928,44 +6893,43 @@
       <c r="A65" s="10">
         <v>64</v>
       </c>
-      <c r="B65" s="35" t="s">
+      <c r="B65" t="s">
         <v>497</v>
       </c>
-      <c r="C65" s="35" t="s">
+      <c r="C65" t="s">
         <v>176</v>
       </c>
-      <c r="D65" s="35" t="s">
+      <c r="D65" t="s">
         <v>42</v>
       </c>
-      <c r="E65" s="35" t="s">
+      <c r="E65" t="s">
         <v>506</v>
       </c>
-      <c r="F65" s="35" t="s">
+      <c r="F65" t="s">
         <v>504</v>
       </c>
-      <c r="G65" s="35"/>
-      <c r="H65" s="35" t="s">
+      <c r="H65" t="s">
         <v>505</v>
       </c>
-      <c r="I65" s="38">
+      <c r="I65" s="2">
         <v>7940</v>
       </c>
-      <c r="J65" s="35" t="s">
+      <c r="J65" t="s">
         <v>499</v>
       </c>
       <c r="K65" s="23" t="s">
         <v>498</v>
       </c>
-      <c r="L65" s="35" t="s">
+      <c r="L65" t="s">
         <v>500</v>
       </c>
-      <c r="M65" s="35" t="s">
+      <c r="M65" t="s">
         <v>501</v>
       </c>
-      <c r="N65" s="35" t="s">
+      <c r="N65" t="s">
         <v>502</v>
       </c>
-      <c r="O65" s="40" t="s">
+      <c r="O65" s="8" t="s">
         <v>422</v>
       </c>
       <c r="P65" s="1" t="s">
@@ -6979,7 +6943,6 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>99</v>
       </c>
-      <c r="S65" s="35"/>
       <c r="T65" t="s">
         <v>701</v>
       </c>
@@ -7507,43 +7470,43 @@
       <c r="A75" s="10">
         <v>74</v>
       </c>
-      <c r="B75" s="35" t="s">
+      <c r="B75" t="s">
         <v>554</v>
       </c>
-      <c r="C75" s="35" t="s">
+      <c r="C75" t="s">
         <v>508</v>
       </c>
-      <c r="D75" s="35" t="s">
+      <c r="D75" t="s">
         <v>20</v>
       </c>
-      <c r="E75" s="35" t="s">
+      <c r="E75" t="s">
         <v>297</v>
       </c>
-      <c r="F75" s="35" t="s">
+      <c r="F75" t="s">
         <v>551</v>
       </c>
-      <c r="G75" s="35" t="s">
+      <c r="G75" t="s">
         <v>552</v>
       </c>
-      <c r="H75" s="35" t="s">
+      <c r="H75" t="s">
         <v>553</v>
       </c>
-      <c r="I75" s="38">
+      <c r="I75" s="2">
         <v>7719</v>
       </c>
-      <c r="J75" s="35" t="s">
+      <c r="J75" t="s">
         <v>550</v>
       </c>
       <c r="K75" s="8" t="s">
         <v>555</v>
       </c>
-      <c r="L75" s="35" t="s">
+      <c r="L75" t="s">
         <v>549</v>
       </c>
-      <c r="M75" s="35" t="s">
+      <c r="M75" t="s">
         <v>562</v>
       </c>
-      <c r="N75" s="35" t="s">
+      <c r="N75" t="s">
         <v>563</v>
       </c>
       <c r="O75" s="8" t="s">
@@ -7560,7 +7523,6 @@
         <f>MID(Table1[[#This Row],[Ages]],FIND("-",Table1[[#This Row],[Ages]])+1,999)</f>
         <v>18</v>
       </c>
-      <c r="S75" s="35"/>
       <c r="T75" t="s">
         <v>744</v>
       </c>
@@ -8385,6 +8347,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Order0 xmlns="bdd75e7b-e8a9-47ee-bfe8-292a25aee042" xsi:nil="true"/>
+    <TaxCatchAll xmlns="416b4836-5b19-40b7-bb16-7007554681d8" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bdd75e7b-e8a9-47ee-bfe8-292a25aee042">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B88086E15D51E443896CF68250FE9008" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="da339e57cb2b25f71630ba83d75a2ac3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bdd75e7b-e8a9-47ee-bfe8-292a25aee042" xmlns:ns3="416b4836-5b19-40b7-bb16-7007554681d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fdb55d46ef9f361b73a98ef20244d266" ns2:_="" ns3:_="">
     <xsd:import namespace="bdd75e7b-e8a9-47ee-bfe8-292a25aee042"/>
@@ -8645,28 +8628,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C85BA7FA-B0CE-44F1-838C-70EF1E91DE8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="bdd75e7b-e8a9-47ee-bfe8-292a25aee042"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="416b4836-5b19-40b7-bb16-7007554681d8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Order0 xmlns="bdd75e7b-e8a9-47ee-bfe8-292a25aee042" xsi:nil="true"/>
-    <TaxCatchAll xmlns="416b4836-5b19-40b7-bb16-7007554681d8" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bdd75e7b-e8a9-47ee-bfe8-292a25aee042">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B187C7C1-0BED-4204-AE89-358C11FEB1FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36CF25E5-8E11-44D1-89DB-617E2E82CFB5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8683,29 +8670,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B187C7C1-0BED-4204-AE89-358C11FEB1FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C85BA7FA-B0CE-44F1-838C-70EF1E91DE8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="bdd75e7b-e8a9-47ee-bfe8-292a25aee042"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="416b4836-5b19-40b7-bb16-7007554681d8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>